<commit_message>
changed excel sheet to aggeregated
</commit_message>
<xml_diff>
--- a/app/assets/images/UES_Sample_Output_V3_9.xlsx
+++ b/app/assets/images/UES_Sample_Output_V3_9.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ukhomeoffice-my.sharepoint.com/personal/ryan_smith5_homeoffice_gov_uk/Documents/Microsoft Teams Chat Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liyaa\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{318797C1-F0CE-4630-B85F-A19CD647EB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC59F908-25FC-4401-B0B5-5EB8366581FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="15600" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -3944,7 +3944,7 @@
     <numFmt numFmtId="164" formatCode="dd\ mmm\ yyyy"/>
     <numFmt numFmtId="165" formatCode="00.00&quot;%&quot;"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4359,6 +4359,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -4374,6 +4375,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4410,8 +4412,6 @@
     <xf numFmtId="0" fontId="5" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5865,42 +5865,42 @@
       <selection activeCell="F1" sqref="F1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.1796875" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="53.85546875" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="24.42578125" customWidth="1"/>
+    <col min="6" max="6" width="53.81640625" customWidth="1"/>
+    <col min="7" max="7" width="22.54296875" customWidth="1"/>
+    <col min="8" max="8" width="16.7265625" customWidth="1"/>
+    <col min="9" max="9" width="24.453125" customWidth="1"/>
     <col min="10" max="10" width="3" customWidth="1"/>
     <col min="11" max="11" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23.25" customHeight="1">
-      <c r="C1" s="35" t="s">
+    <row r="1" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="34" t="s">
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="34"/>
-    </row>
-    <row r="2" spans="1:10" ht="41.25" customHeight="1">
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35" t="s">
+      <c r="G1" s="35"/>
+    </row>
+    <row r="2" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="35"/>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="G2" s="36"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -5912,23 +5912,23 @@
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
     </row>
-    <row r="5" spans="1:10" ht="26.45" customHeight="1">
-      <c r="B5" s="50" t="s">
+    <row r="5" spans="1:10" ht="26.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-    </row>
-    <row r="6" spans="1:10" ht="60.95" customHeight="1">
-      <c r="B6" s="33" t="s">
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+    </row>
+    <row r="6" spans="1:10" ht="61" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="33"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="32" t="s">
         <v>2</v>
       </c>
@@ -5942,11 +5942,11 @@
       </c>
       <c r="I6" s="32"/>
     </row>
-    <row r="7" spans="1:10" ht="53.1" customHeight="1">
-      <c r="B7" s="33" t="s">
+    <row r="7" spans="1:10" ht="53.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="33"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="32"/>
       <c r="E7" s="32"/>
       <c r="F7" s="32"/>
@@ -5958,11 +5958,11 @@
       </c>
       <c r="I7" s="32"/>
     </row>
-    <row r="8" spans="1:10" ht="45" customHeight="1">
-      <c r="B8" s="33" t="s">
+    <row r="8" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="33"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="32"/>
       <c r="E8" s="32"/>
       <c r="F8" s="32"/>
@@ -5974,19 +5974,19 @@
       </c>
       <c r="I8" s="32"/>
     </row>
-    <row r="10" spans="1:10" ht="20.25">
-      <c r="B10" s="50" t="s">
+    <row r="10" spans="1:10" ht="20" x14ac:dyDescent="0.4">
+      <c r="B10" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="50"/>
-      <c r="I10" s="50"/>
-    </row>
-    <row r="11" spans="1:10" ht="63" customHeight="1">
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+    </row>
+    <row r="11" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="26" t="s">
         <v>14</v>
       </c>
@@ -6000,7 +6000,7 @@
       <c r="H11" s="32"/>
       <c r="I11" s="32"/>
     </row>
-    <row r="12" spans="1:10" ht="39.950000000000003" customHeight="1">
+    <row r="12" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="26" t="s">
         <v>16</v>
       </c>
@@ -6014,7 +6014,7 @@
       <c r="H12" s="32"/>
       <c r="I12" s="32"/>
     </row>
-    <row r="13" spans="1:10" ht="39" customHeight="1">
+    <row r="13" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="26" t="s">
         <v>18</v>
       </c>
@@ -6028,7 +6028,7 @@
       <c r="H13" s="32"/>
       <c r="I13" s="32"/>
     </row>
-    <row r="14" spans="1:10" ht="68.45" customHeight="1">
+    <row r="14" spans="1:10" ht="68.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="26" t="s">
         <v>19</v>
       </c>
@@ -6042,59 +6042,59 @@
       <c r="H14" s="32"/>
       <c r="I14" s="32"/>
     </row>
-    <row r="15" spans="1:10" ht="39.950000000000003" customHeight="1"/>
-    <row r="16" spans="1:10" ht="20.45" customHeight="1">
-      <c r="B16" s="50" t="s">
+    <row r="15" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:10" ht="20.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="50"/>
-    </row>
-    <row r="17" spans="2:9" ht="409.5" customHeight="1">
-      <c r="B17" s="36" t="s">
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+    </row>
+    <row r="17" spans="2:9" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
-    </row>
-    <row r="18" spans="2:9" ht="18" customHeight="1"/>
-    <row r="19" spans="2:9" ht="20.25">
-      <c r="B19" s="50" t="s">
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+    </row>
+    <row r="18" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="2:9" ht="20" x14ac:dyDescent="0.4">
+      <c r="B19" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="50"/>
-    </row>
-    <row r="20" spans="2:9" ht="31.5" customHeight="1">
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+    </row>
+    <row r="20" spans="2:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="37" t="s">
+      <c r="C20" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="37"/>
-    </row>
-    <row r="21" spans="2:9" ht="312" customHeight="1">
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+    </row>
+    <row r="21" spans="2:9" ht="312" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="26" t="s">
         <v>26</v>
       </c>
@@ -6108,10 +6108,10 @@
       <c r="H21" s="32"/>
       <c r="I21" s="32"/>
     </row>
-    <row r="22" spans="2:9" ht="31.5" customHeight="1"/>
-    <row r="25" spans="2:9" ht="408.95" customHeight="1"/>
-    <row r="28" spans="2:9" ht="26.25" customHeight="1"/>
-    <row r="29" spans="2:9" ht="189.95" customHeight="1"/>
+    <row r="22" spans="2:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="2:9" ht="409" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="2:9" ht="190" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="23">
     <mergeCell ref="C13:I13"/>
@@ -6163,36 +6163,36 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1"/>
-    <col min="7" max="8" width="15.7109375" customWidth="1"/>
-    <col min="9" max="9" width="110.7109375" customWidth="1"/>
-    <col min="10" max="10" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" customWidth="1"/>
+    <col min="3" max="3" width="30.7265625" customWidth="1"/>
+    <col min="4" max="5" width="15.7265625" customWidth="1"/>
+    <col min="6" max="6" width="19.26953125" customWidth="1"/>
+    <col min="7" max="8" width="15.7265625" customWidth="1"/>
+    <col min="9" max="9" width="110.7265625" customWidth="1"/>
+    <col min="10" max="10" width="2.7265625" customWidth="1"/>
     <col min="11" max="11" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23.25" customHeight="1">
-      <c r="C1" s="35" t="s">
+    <row r="1" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="35"/>
+      <c r="D1" s="36"/>
       <c r="F1" s="19" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="56.45" customHeight="1">
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
+    <row r="2" spans="1:10" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
       <c r="F2" s="20" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="21.95" customHeight="1">
+    <row r="3" spans="1:10" ht="22" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -6204,31 +6204,31 @@
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
     </row>
-    <row r="5" spans="1:10" ht="18">
-      <c r="B5" s="51" t="s">
+    <row r="5" spans="1:10" ht="18" x14ac:dyDescent="0.4">
+      <c r="B5" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="B6" s="36" t="s">
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-    </row>
-    <row r="8" spans="1:10" ht="25.5">
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+    </row>
+    <row r="8" spans="1:10" ht="26" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>30</v>
       </c>
@@ -6254,7 +6254,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="25.5">
+    <row r="9" spans="1:10" ht="25" x14ac:dyDescent="0.35">
       <c r="B9" s="5" t="s">
         <v>38</v>
       </c>
@@ -6280,7 +6280,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
         <v>41</v>
       </c>
@@ -6306,7 +6306,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B11" s="5" t="s">
         <v>44</v>
       </c>
@@ -6332,7 +6332,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="25.5">
+    <row r="12" spans="1:10" ht="25" x14ac:dyDescent="0.35">
       <c r="B12" s="5" t="s">
         <v>47</v>
       </c>
@@ -6358,7 +6358,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="25.5">
+    <row r="13" spans="1:10" ht="25" x14ac:dyDescent="0.35">
       <c r="B13" s="5" t="s">
         <v>50</v>
       </c>
@@ -6384,7 +6384,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B14" s="5" t="s">
         <v>53</v>
       </c>
@@ -6410,7 +6410,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B15" s="5" t="s">
         <v>56</v>
       </c>
@@ -6436,7 +6436,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B16" s="5" t="s">
         <v>59</v>
       </c>
@@ -6462,7 +6462,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="25.5">
+    <row r="17" spans="2:9" ht="25" x14ac:dyDescent="0.35">
       <c r="B17" s="5" t="s">
         <v>62</v>
       </c>
@@ -6488,7 +6488,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="25.5">
+    <row r="18" spans="2:9" ht="25" x14ac:dyDescent="0.35">
       <c r="B18" s="5" t="s">
         <v>65</v>
       </c>
@@ -6514,7 +6514,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="25.5">
+    <row r="19" spans="2:9" ht="25" x14ac:dyDescent="0.35">
       <c r="B19" s="5" t="s">
         <v>68</v>
       </c>
@@ -6540,7 +6540,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="2:9">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B20" s="5" t="s">
         <v>71</v>
       </c>
@@ -6566,7 +6566,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="25.5">
+    <row r="21" spans="2:9" ht="25" x14ac:dyDescent="0.35">
       <c r="B21" s="5" t="s">
         <v>74</v>
       </c>
@@ -6592,7 +6592,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="2:9">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B22" s="5" t="s">
         <v>77</v>
       </c>
@@ -6614,7 +6614,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="25.5">
+    <row r="23" spans="2:9" ht="25" x14ac:dyDescent="0.35">
       <c r="B23" s="5" t="s">
         <v>80</v>
       </c>
@@ -6640,7 +6640,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="2:9">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B24" s="5" t="s">
         <v>83</v>
       </c>
@@ -6662,7 +6662,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="2:9">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B25" s="5" t="s">
         <v>86</v>
       </c>
@@ -6688,7 +6688,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="2:9" ht="25.5">
+    <row r="26" spans="2:9" ht="25" x14ac:dyDescent="0.35">
       <c r="B26" s="5" t="s">
         <v>89</v>
       </c>
@@ -6714,7 +6714,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="2:9">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B27" s="5" t="s">
         <v>92</v>
       </c>
@@ -6736,7 +6736,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="2:9">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B28" s="5" t="s">
         <v>95</v>
       </c>
@@ -6762,7 +6762,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="2:9">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B29" s="5" t="s">
         <v>98</v>
       </c>
@@ -6788,7 +6788,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="2:9">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B30" s="5" t="s">
         <v>101</v>
       </c>
@@ -6814,7 +6814,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="2:9">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B31" s="5" t="s">
         <v>104</v>
       </c>
@@ -6840,7 +6840,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="2:9" ht="38.25">
+    <row r="32" spans="2:9" ht="25" x14ac:dyDescent="0.35">
       <c r="B32" s="5" t="s">
         <v>107</v>
       </c>
@@ -6891,126 +6891,126 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AZ4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="AU3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="AI3" sqref="AI3"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" customWidth="1"/>
-    <col min="3" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="31.5703125" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" customWidth="1"/>
-    <col min="9" max="9" width="40.7109375" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" customWidth="1"/>
-    <col min="12" max="12" width="40.7109375" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" customWidth="1"/>
-    <col min="14" max="15" width="7.7109375" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" customWidth="1"/>
-    <col min="17" max="17" width="16.7109375" customWidth="1"/>
-    <col min="18" max="18" width="19.7109375" customWidth="1"/>
-    <col min="19" max="19" width="20.7109375" customWidth="1"/>
-    <col min="20" max="20" width="32.7109375" customWidth="1"/>
-    <col min="21" max="21" width="50.7109375" customWidth="1"/>
-    <col min="22" max="22" width="13.7109375" customWidth="1"/>
-    <col min="23" max="23" width="16.7109375" customWidth="1"/>
-    <col min="24" max="24" width="13.7109375" customWidth="1"/>
-    <col min="25" max="25" width="60.7109375" customWidth="1"/>
-    <col min="26" max="26" width="25.7109375" customWidth="1"/>
-    <col min="27" max="27" width="60.7109375" customWidth="1"/>
-    <col min="28" max="28" width="54.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="52.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.7109375" customWidth="1"/>
-    <col min="32" max="32" width="80.7109375" customWidth="1"/>
-    <col min="33" max="34" width="20.7109375" customWidth="1"/>
-    <col min="35" max="35" width="80.7109375" customWidth="1"/>
-    <col min="36" max="36" width="50.7109375" customWidth="1"/>
-    <col min="37" max="38" width="150.7109375" customWidth="1"/>
-    <col min="39" max="39" width="40.7109375" customWidth="1"/>
-    <col min="40" max="40" width="20.7109375" customWidth="1"/>
-    <col min="41" max="41" width="80.7109375" customWidth="1"/>
-    <col min="42" max="42" width="40.7109375" customWidth="1"/>
-    <col min="43" max="43" width="100.7109375" customWidth="1"/>
-    <col min="44" max="45" width="80.7109375" customWidth="1"/>
-    <col min="46" max="50" width="20.7109375" customWidth="1"/>
-    <col min="51" max="52" width="80.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.81640625" customWidth="1"/>
+    <col min="3" max="4" width="12.7265625" customWidth="1"/>
+    <col min="5" max="5" width="31.54296875" customWidth="1"/>
+    <col min="6" max="6" width="20.7265625" customWidth="1"/>
+    <col min="7" max="7" width="10.7265625" customWidth="1"/>
+    <col min="8" max="8" width="20.7265625" customWidth="1"/>
+    <col min="9" max="9" width="40.7265625" customWidth="1"/>
+    <col min="10" max="10" width="10.7265625" customWidth="1"/>
+    <col min="11" max="11" width="8.7265625" customWidth="1"/>
+    <col min="12" max="12" width="40.7265625" customWidth="1"/>
+    <col min="13" max="13" width="14.7265625" customWidth="1"/>
+    <col min="14" max="15" width="7.7265625" customWidth="1"/>
+    <col min="16" max="16" width="10.7265625" customWidth="1"/>
+    <col min="17" max="17" width="16.7265625" customWidth="1"/>
+    <col min="18" max="18" width="19.7265625" customWidth="1"/>
+    <col min="19" max="19" width="20.7265625" customWidth="1"/>
+    <col min="20" max="20" width="32.7265625" customWidth="1"/>
+    <col min="21" max="21" width="50.7265625" customWidth="1"/>
+    <col min="22" max="22" width="13.7265625" customWidth="1"/>
+    <col min="23" max="23" width="16.7265625" customWidth="1"/>
+    <col min="24" max="24" width="13.7265625" customWidth="1"/>
+    <col min="25" max="25" width="60.7265625" customWidth="1"/>
+    <col min="26" max="26" width="25.7265625" customWidth="1"/>
+    <col min="27" max="27" width="60.7265625" customWidth="1"/>
+    <col min="28" max="28" width="54.453125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="52.453125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="33.54296875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.7265625" customWidth="1"/>
+    <col min="32" max="32" width="80.7265625" customWidth="1"/>
+    <col min="33" max="34" width="20.7265625" customWidth="1"/>
+    <col min="35" max="35" width="80.7265625" customWidth="1"/>
+    <col min="36" max="36" width="50.7265625" customWidth="1"/>
+    <col min="37" max="38" width="150.7265625" customWidth="1"/>
+    <col min="39" max="39" width="40.7265625" customWidth="1"/>
+    <col min="40" max="40" width="20.7265625" customWidth="1"/>
+    <col min="41" max="41" width="80.7265625" customWidth="1"/>
+    <col min="42" max="42" width="40.7265625" customWidth="1"/>
+    <col min="43" max="43" width="100.7265625" customWidth="1"/>
+    <col min="44" max="45" width="80.7265625" customWidth="1"/>
+    <col min="46" max="50" width="20.7265625" customWidth="1"/>
+    <col min="51" max="52" width="80.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="23.25">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:52" ht="23" x14ac:dyDescent="0.5">
+      <c r="A1" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="42" t="s">
+      <c r="B1" s="43"/>
+      <c r="C1" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="43" t="s">
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="44"/>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="45"/>
-      <c r="Y1" s="46" t="s">
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="46"/>
+      <c r="V1" s="46"/>
+      <c r="W1" s="46"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="46"/>
-      <c r="AB1" s="47" t="s">
+      <c r="Z1" s="48"/>
+      <c r="AA1" s="48"/>
+      <c r="AB1" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="AC1" s="47"/>
-      <c r="AD1" s="47"/>
-      <c r="AE1" s="47"/>
-      <c r="AF1" s="38" t="s">
+      <c r="AC1" s="49"/>
+      <c r="AD1" s="49"/>
+      <c r="AE1" s="49"/>
+      <c r="AF1" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="AG1" s="38"/>
-      <c r="AH1" s="38"/>
-      <c r="AI1" s="38"/>
-      <c r="AJ1" s="38"/>
-      <c r="AK1" s="39" t="s">
+      <c r="AG1" s="40"/>
+      <c r="AH1" s="40"/>
+      <c r="AI1" s="40"/>
+      <c r="AJ1" s="40"/>
+      <c r="AK1" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="AL1" s="39"/>
-      <c r="AM1" s="39"/>
-      <c r="AN1" s="39"/>
-      <c r="AO1" s="39"/>
-      <c r="AP1" s="39"/>
-      <c r="AQ1" s="39"/>
-      <c r="AR1" s="39"/>
-      <c r="AS1" s="39"/>
-      <c r="AT1" s="39"/>
-      <c r="AU1" s="39"/>
-      <c r="AV1" s="40" t="s">
+      <c r="AL1" s="41"/>
+      <c r="AM1" s="41"/>
+      <c r="AN1" s="41"/>
+      <c r="AO1" s="41"/>
+      <c r="AP1" s="41"/>
+      <c r="AQ1" s="41"/>
+      <c r="AR1" s="41"/>
+      <c r="AS1" s="41"/>
+      <c r="AT1" s="41"/>
+      <c r="AU1" s="41"/>
+      <c r="AV1" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="AW1" s="40"/>
-      <c r="AX1" s="40"/>
+      <c r="AW1" s="42"/>
+      <c r="AX1" s="42"/>
       <c r="AY1" s="22" t="s">
         <v>118</v>
       </c>
@@ -7018,7 +7018,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:52" ht="30" customHeight="1">
+    <row r="2" spans="1:52" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>120</v>
       </c>
@@ -7176,7 +7176,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:52" ht="280.5">
+    <row r="3" spans="1:52" ht="262.5" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
         <v>169</v>
       </c>
@@ -7330,7 +7330,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="4" spans="1:52">
+    <row r="4" spans="1:52" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>210</v>
       </c>
@@ -7512,200 +7512,200 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:CP35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="AZ11" sqref="AZ11"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="5" width="12.7109375" customWidth="1"/>
-    <col min="6" max="16" width="10.7109375" customWidth="1"/>
-    <col min="17" max="17" width="20.7109375" customWidth="1"/>
-    <col min="18" max="18" width="40.7109375" customWidth="1"/>
-    <col min="19" max="19" width="10.7109375" customWidth="1"/>
-    <col min="20" max="20" width="20.7109375" customWidth="1"/>
-    <col min="21" max="21" width="40.7109375" customWidth="1"/>
-    <col min="22" max="22" width="96.28515625" customWidth="1"/>
-    <col min="23" max="23" width="40.7109375" customWidth="1"/>
-    <col min="24" max="24" width="10.7109375" customWidth="1"/>
-    <col min="25" max="25" width="8.7109375" customWidth="1"/>
-    <col min="26" max="26" width="40.7109375" customWidth="1"/>
-    <col min="27" max="27" width="14.7109375" customWidth="1"/>
-    <col min="28" max="29" width="7.7109375" customWidth="1"/>
-    <col min="30" max="30" width="10.7109375" customWidth="1"/>
-    <col min="31" max="31" width="16.7109375" customWidth="1"/>
-    <col min="32" max="32" width="19.7109375" customWidth="1"/>
-    <col min="33" max="33" width="20.7109375" customWidth="1"/>
-    <col min="34" max="34" width="32.7109375" customWidth="1"/>
-    <col min="35" max="36" width="20.7109375" customWidth="1"/>
-    <col min="37" max="37" width="50.7109375" customWidth="1"/>
-    <col min="38" max="38" width="13.7109375" customWidth="1"/>
-    <col min="39" max="39" width="16.7109375" customWidth="1"/>
-    <col min="40" max="40" width="13.7109375" customWidth="1"/>
-    <col min="41" max="41" width="60.7109375" customWidth="1"/>
-    <col min="42" max="42" width="25.7109375" customWidth="1"/>
-    <col min="43" max="43" width="60.7109375" customWidth="1"/>
-    <col min="44" max="45" width="100.7109375" customWidth="1"/>
-    <col min="46" max="46" width="35.7109375" customWidth="1"/>
-    <col min="47" max="47" width="10.7109375" customWidth="1"/>
-    <col min="48" max="48" width="15.7109375" customWidth="1"/>
-    <col min="49" max="49" width="11.7109375" customWidth="1"/>
-    <col min="50" max="50" width="23.7109375" customWidth="1"/>
-    <col min="51" max="51" width="11.7109375" customWidth="1"/>
-    <col min="52" max="52" width="23.7109375" customWidth="1"/>
-    <col min="53" max="53" width="15.7109375" customWidth="1"/>
-    <col min="54" max="54" width="14.7109375" customWidth="1"/>
-    <col min="55" max="57" width="20.7109375" customWidth="1"/>
-    <col min="58" max="58" width="80.7109375" customWidth="1"/>
-    <col min="59" max="62" width="20.7109375" customWidth="1"/>
-    <col min="63" max="63" width="14.7109375" customWidth="1"/>
-    <col min="64" max="65" width="35.7109375" customWidth="1"/>
-    <col min="66" max="67" width="14.7109375" customWidth="1"/>
-    <col min="68" max="69" width="40.7109375" customWidth="1"/>
-    <col min="70" max="70" width="10.7109375" customWidth="1"/>
-    <col min="71" max="71" width="14.7109375" customWidth="1"/>
-    <col min="72" max="72" width="150.7109375" customWidth="1"/>
-    <col min="73" max="73" width="40.7109375" customWidth="1"/>
-    <col min="74" max="74" width="20.7109375" customWidth="1"/>
-    <col min="75" max="75" width="80.7109375" customWidth="1"/>
-    <col min="76" max="76" width="40.7109375" customWidth="1"/>
-    <col min="77" max="77" width="100.7109375" customWidth="1"/>
-    <col min="78" max="79" width="80.7109375" customWidth="1"/>
-    <col min="80" max="84" width="20.7109375" customWidth="1"/>
-    <col min="85" max="85" width="15.140625" customWidth="1"/>
-    <col min="86" max="86" width="16.5703125" customWidth="1"/>
-    <col min="87" max="87" width="40.7109375" customWidth="1"/>
-    <col min="88" max="88" width="50.7109375" customWidth="1"/>
-    <col min="89" max="89" width="80.7109375" customWidth="1"/>
-    <col min="90" max="90" width="18.7109375" customWidth="1"/>
-    <col min="91" max="91" width="12.7109375" customWidth="1"/>
-    <col min="92" max="93" width="20.7109375" customWidth="1"/>
-    <col min="94" max="94" width="80.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" customWidth="1"/>
+    <col min="4" max="5" width="12.7265625" customWidth="1"/>
+    <col min="6" max="16" width="10.7265625" customWidth="1"/>
+    <col min="17" max="17" width="20.7265625" customWidth="1"/>
+    <col min="18" max="18" width="40.7265625" customWidth="1"/>
+    <col min="19" max="19" width="10.7265625" customWidth="1"/>
+    <col min="20" max="20" width="20.7265625" customWidth="1"/>
+    <col min="21" max="21" width="40.7265625" customWidth="1"/>
+    <col min="22" max="22" width="96.26953125" customWidth="1"/>
+    <col min="23" max="23" width="40.7265625" customWidth="1"/>
+    <col min="24" max="24" width="10.7265625" customWidth="1"/>
+    <col min="25" max="25" width="8.7265625" customWidth="1"/>
+    <col min="26" max="26" width="40.7265625" customWidth="1"/>
+    <col min="27" max="27" width="14.7265625" customWidth="1"/>
+    <col min="28" max="29" width="7.7265625" customWidth="1"/>
+    <col min="30" max="30" width="10.7265625" customWidth="1"/>
+    <col min="31" max="31" width="16.7265625" customWidth="1"/>
+    <col min="32" max="32" width="19.7265625" customWidth="1"/>
+    <col min="33" max="33" width="20.7265625" customWidth="1"/>
+    <col min="34" max="34" width="32.7265625" customWidth="1"/>
+    <col min="35" max="36" width="20.7265625" customWidth="1"/>
+    <col min="37" max="37" width="50.7265625" customWidth="1"/>
+    <col min="38" max="38" width="13.7265625" customWidth="1"/>
+    <col min="39" max="39" width="16.7265625" customWidth="1"/>
+    <col min="40" max="40" width="13.7265625" customWidth="1"/>
+    <col min="41" max="41" width="60.7265625" customWidth="1"/>
+    <col min="42" max="42" width="25.7265625" customWidth="1"/>
+    <col min="43" max="43" width="60.7265625" customWidth="1"/>
+    <col min="44" max="45" width="100.7265625" customWidth="1"/>
+    <col min="46" max="46" width="35.7265625" customWidth="1"/>
+    <col min="47" max="47" width="10.7265625" customWidth="1"/>
+    <col min="48" max="48" width="15.7265625" customWidth="1"/>
+    <col min="49" max="49" width="11.7265625" customWidth="1"/>
+    <col min="50" max="50" width="23.7265625" customWidth="1"/>
+    <col min="51" max="51" width="11.7265625" customWidth="1"/>
+    <col min="52" max="52" width="23.7265625" customWidth="1"/>
+    <col min="53" max="53" width="15.7265625" customWidth="1"/>
+    <col min="54" max="54" width="14.7265625" customWidth="1"/>
+    <col min="55" max="57" width="20.7265625" customWidth="1"/>
+    <col min="58" max="58" width="80.7265625" customWidth="1"/>
+    <col min="59" max="62" width="20.7265625" customWidth="1"/>
+    <col min="63" max="63" width="14.7265625" customWidth="1"/>
+    <col min="64" max="65" width="35.7265625" customWidth="1"/>
+    <col min="66" max="67" width="14.7265625" customWidth="1"/>
+    <col min="68" max="69" width="40.7265625" customWidth="1"/>
+    <col min="70" max="70" width="10.7265625" customWidth="1"/>
+    <col min="71" max="71" width="14.7265625" customWidth="1"/>
+    <col min="72" max="72" width="150.7265625" customWidth="1"/>
+    <col min="73" max="73" width="40.7265625" customWidth="1"/>
+    <col min="74" max="74" width="20.7265625" customWidth="1"/>
+    <col min="75" max="75" width="80.7265625" customWidth="1"/>
+    <col min="76" max="76" width="40.7265625" customWidth="1"/>
+    <col min="77" max="77" width="100.7265625" customWidth="1"/>
+    <col min="78" max="79" width="80.7265625" customWidth="1"/>
+    <col min="80" max="84" width="20.7265625" customWidth="1"/>
+    <col min="85" max="85" width="15.1796875" customWidth="1"/>
+    <col min="86" max="86" width="16.54296875" customWidth="1"/>
+    <col min="87" max="87" width="40.7265625" customWidth="1"/>
+    <col min="88" max="88" width="50.7265625" customWidth="1"/>
+    <col min="89" max="89" width="80.7265625" customWidth="1"/>
+    <col min="90" max="90" width="18.7265625" customWidth="1"/>
+    <col min="91" max="91" width="12.7265625" customWidth="1"/>
+    <col min="92" max="93" width="20.7265625" customWidth="1"/>
+    <col min="94" max="94" width="80.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:94" ht="23.25">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:94" ht="23" x14ac:dyDescent="0.5">
+      <c r="A1" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="42" t="s">
+      <c r="B1" s="43"/>
+      <c r="C1" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42"/>
-      <c r="S1" s="42"/>
-      <c r="T1" s="42"/>
-      <c r="U1" s="42"/>
-      <c r="V1" s="42"/>
-      <c r="W1" s="42"/>
-      <c r="X1" s="42"/>
-      <c r="Y1" s="48" t="s">
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="Z1" s="48"/>
-      <c r="AA1" s="48"/>
-      <c r="AB1" s="48"/>
-      <c r="AC1" s="48"/>
-      <c r="AD1" s="48"/>
-      <c r="AE1" s="48"/>
-      <c r="AF1" s="48"/>
-      <c r="AG1" s="48"/>
-      <c r="AH1" s="48"/>
-      <c r="AI1" s="48"/>
-      <c r="AJ1" s="48"/>
-      <c r="AK1" s="48"/>
-      <c r="AL1" s="48"/>
-      <c r="AM1" s="48"/>
-      <c r="AN1" s="48"/>
-      <c r="AO1" s="46" t="s">
+      <c r="Z1" s="50"/>
+      <c r="AA1" s="50"/>
+      <c r="AB1" s="50"/>
+      <c r="AC1" s="50"/>
+      <c r="AD1" s="50"/>
+      <c r="AE1" s="50"/>
+      <c r="AF1" s="50"/>
+      <c r="AG1" s="50"/>
+      <c r="AH1" s="50"/>
+      <c r="AI1" s="50"/>
+      <c r="AJ1" s="50"/>
+      <c r="AK1" s="50"/>
+      <c r="AL1" s="50"/>
+      <c r="AM1" s="50"/>
+      <c r="AN1" s="50"/>
+      <c r="AO1" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="AP1" s="46"/>
-      <c r="AQ1" s="46"/>
-      <c r="AR1" s="47" t="s">
+      <c r="AP1" s="48"/>
+      <c r="AQ1" s="48"/>
+      <c r="AR1" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="AS1" s="47"/>
-      <c r="AT1" s="47"/>
-      <c r="AU1" s="47"/>
-      <c r="AV1" s="38" t="s">
+      <c r="AS1" s="49"/>
+      <c r="AT1" s="49"/>
+      <c r="AU1" s="49"/>
+      <c r="AV1" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="AW1" s="38"/>
-      <c r="AX1" s="38"/>
-      <c r="AY1" s="38"/>
-      <c r="AZ1" s="38"/>
-      <c r="BA1" s="38"/>
-      <c r="BB1" s="38"/>
-      <c r="BC1" s="38"/>
-      <c r="BD1" s="38"/>
-      <c r="BE1" s="38"/>
-      <c r="BF1" s="38"/>
-      <c r="BG1" s="38"/>
-      <c r="BH1" s="38"/>
-      <c r="BI1" s="38"/>
-      <c r="BJ1" s="38"/>
-      <c r="BK1" s="39" t="s">
+      <c r="AW1" s="40"/>
+      <c r="AX1" s="40"/>
+      <c r="AY1" s="40"/>
+      <c r="AZ1" s="40"/>
+      <c r="BA1" s="40"/>
+      <c r="BB1" s="40"/>
+      <c r="BC1" s="40"/>
+      <c r="BD1" s="40"/>
+      <c r="BE1" s="40"/>
+      <c r="BF1" s="40"/>
+      <c r="BG1" s="40"/>
+      <c r="BH1" s="40"/>
+      <c r="BI1" s="40"/>
+      <c r="BJ1" s="40"/>
+      <c r="BK1" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="BL1" s="39"/>
-      <c r="BM1" s="39"/>
-      <c r="BN1" s="39"/>
-      <c r="BO1" s="39"/>
-      <c r="BP1" s="39"/>
-      <c r="BQ1" s="39"/>
-      <c r="BR1" s="39"/>
-      <c r="BS1" s="39"/>
-      <c r="BT1" s="39"/>
-      <c r="BU1" s="39"/>
-      <c r="BV1" s="39"/>
-      <c r="BW1" s="39"/>
-      <c r="BX1" s="39"/>
-      <c r="BY1" s="39"/>
-      <c r="BZ1" s="39"/>
-      <c r="CA1" s="39"/>
-      <c r="CB1" s="39"/>
-      <c r="CC1" s="39"/>
-      <c r="CD1" s="40" t="s">
+      <c r="BL1" s="41"/>
+      <c r="BM1" s="41"/>
+      <c r="BN1" s="41"/>
+      <c r="BO1" s="41"/>
+      <c r="BP1" s="41"/>
+      <c r="BQ1" s="41"/>
+      <c r="BR1" s="41"/>
+      <c r="BS1" s="41"/>
+      <c r="BT1" s="41"/>
+      <c r="BU1" s="41"/>
+      <c r="BV1" s="41"/>
+      <c r="BW1" s="41"/>
+      <c r="BX1" s="41"/>
+      <c r="BY1" s="41"/>
+      <c r="BZ1" s="41"/>
+      <c r="CA1" s="41"/>
+      <c r="CB1" s="41"/>
+      <c r="CC1" s="41"/>
+      <c r="CD1" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="CE1" s="40"/>
-      <c r="CF1" s="40"/>
-      <c r="CG1" s="40" t="s">
+      <c r="CE1" s="42"/>
+      <c r="CF1" s="42"/>
+      <c r="CG1" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="CH1" s="40"/>
-      <c r="CI1" s="40"/>
-      <c r="CJ1" s="40"/>
-      <c r="CK1" s="40"/>
-      <c r="CL1" s="40" t="s">
+      <c r="CH1" s="42"/>
+      <c r="CI1" s="42"/>
+      <c r="CJ1" s="42"/>
+      <c r="CK1" s="42"/>
+      <c r="CL1" s="42" t="s">
         <v>212</v>
       </c>
-      <c r="CM1" s="40"/>
-      <c r="CN1" s="40"/>
-      <c r="CO1" s="40"/>
-      <c r="CP1" s="40"/>
-    </row>
-    <row r="2" spans="1:94" ht="39.75" thickBot="1">
+      <c r="CM1" s="42"/>
+      <c r="CN1" s="42"/>
+      <c r="CO1" s="42"/>
+      <c r="CP1" s="42"/>
+    </row>
+    <row r="2" spans="1:94" ht="40" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="10" t="s">
         <v>120</v>
       </c>
@@ -7989,7 +7989,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:94" ht="129" thickTop="1" thickBot="1">
+    <row r="3" spans="1:94" ht="163.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="9" t="s">
         <v>169</v>
       </c>
@@ -8233,7 +8233,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:94" ht="129" thickTop="1" thickBot="1">
+    <row r="4" spans="1:94" ht="163.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
         <v>169</v>
       </c>
@@ -8450,7 +8450,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:94" ht="128.25" thickBot="1">
+    <row r="5" spans="1:94" ht="163" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
         <v>169</v>
       </c>
@@ -8692,7 +8692,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="1:94" ht="128.25" thickBot="1">
+    <row r="6" spans="1:94" ht="163" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
         <v>169</v>
       </c>
@@ -8912,7 +8912,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="7" spans="1:94" ht="115.5" thickBot="1">
+    <row r="7" spans="1:94" ht="163" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
         <v>169</v>
       </c>
@@ -9136,7 +9136,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="8" spans="1:94" ht="115.5" thickBot="1">
+    <row r="8" spans="1:94" ht="163" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
         <v>169</v>
       </c>
@@ -9360,7 +9360,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="9" spans="1:94" ht="116.25" thickTop="1" thickBot="1">
+    <row r="9" spans="1:94" ht="163.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>169</v>
       </c>
@@ -9580,7 +9580,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="10" spans="1:94" ht="116.25" thickTop="1" thickBot="1">
+    <row r="10" spans="1:94" ht="163.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>169</v>
       </c>
@@ -9818,7 +9818,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="11" spans="1:94" ht="116.25" thickTop="1" thickBot="1">
+    <row r="11" spans="1:94" ht="163.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="31" t="s">
         <v>169</v>
       </c>
@@ -10056,7 +10056,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="12" spans="1:94" ht="116.25" thickTop="1" thickBot="1">
+    <row r="12" spans="1:94" ht="163.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="31" t="s">
         <v>169</v>
       </c>
@@ -10294,7 +10294,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="13" spans="1:94" ht="116.25" thickTop="1" thickBot="1">
+    <row r="13" spans="1:94" ht="163.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
         <v>169</v>
       </c>
@@ -10524,7 +10524,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="14" spans="1:94" ht="116.25" thickTop="1" thickBot="1">
+    <row r="14" spans="1:94" ht="163.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
         <v>169</v>
       </c>
@@ -10756,7 +10756,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="15" spans="1:94" ht="15.75" thickTop="1">
+    <row r="15" spans="1:94" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>210</v>
       </c>
@@ -11026,7 +11026,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="16" spans="1:94">
+    <row r="16" spans="1:94" x14ac:dyDescent="0.35">
       <c r="V16" s="12"/>
       <c r="W16" s="5" t="s">
         <v>181</v>
@@ -11071,7 +11071,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="17" spans="23:94">
+    <row r="17" spans="23:94" x14ac:dyDescent="0.35">
       <c r="W17" s="5" t="s">
         <v>181</v>
       </c>
@@ -11115,7 +11115,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="18" spans="23:94" ht="51">
+    <row r="18" spans="23:94" ht="50" x14ac:dyDescent="0.35">
       <c r="W18" s="5" t="s">
         <v>181</v>
       </c>
@@ -11159,7 +11159,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="19" spans="23:94">
+    <row r="19" spans="23:94" x14ac:dyDescent="0.35">
       <c r="W19" s="5" t="s">
         <v>181</v>
       </c>
@@ -11203,7 +11203,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="20" spans="23:94">
+    <row r="20" spans="23:94" x14ac:dyDescent="0.35">
       <c r="W20" s="5" t="s">
         <v>181</v>
       </c>
@@ -11247,7 +11247,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="21" spans="23:94">
+    <row r="21" spans="23:94" x14ac:dyDescent="0.35">
       <c r="W21" s="5" t="s">
         <v>181</v>
       </c>
@@ -11291,7 +11291,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="22" spans="23:94">
+    <row r="22" spans="23:94" x14ac:dyDescent="0.35">
       <c r="W22" s="5" t="s">
         <v>181</v>
       </c>
@@ -11335,7 +11335,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="23" spans="23:94">
+    <row r="23" spans="23:94" x14ac:dyDescent="0.35">
       <c r="W23" s="5" t="s">
         <v>181</v>
       </c>
@@ -11379,7 +11379,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="24" spans="23:94" ht="102">
+    <row r="24" spans="23:94" ht="87.5" x14ac:dyDescent="0.35">
       <c r="W24" s="5" t="s">
         <v>181</v>
       </c>
@@ -11423,7 +11423,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="25" spans="23:94">
+    <row r="25" spans="23:94" x14ac:dyDescent="0.35">
       <c r="W25" s="5" t="s">
         <v>181</v>
       </c>
@@ -11467,7 +11467,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="26" spans="23:94">
+    <row r="26" spans="23:94" x14ac:dyDescent="0.35">
       <c r="W26" s="5" t="s">
         <v>181</v>
       </c>
@@ -11511,7 +11511,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="27" spans="23:94" ht="63.75">
+    <row r="27" spans="23:94" ht="62.5" x14ac:dyDescent="0.35">
       <c r="W27" s="5" t="s">
         <v>181</v>
       </c>
@@ -11555,7 +11555,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="28" spans="23:94">
+    <row r="28" spans="23:94" x14ac:dyDescent="0.35">
       <c r="W28" s="5" t="s">
         <v>181</v>
       </c>
@@ -11599,7 +11599,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="29" spans="23:94">
+    <row r="29" spans="23:94" x14ac:dyDescent="0.35">
       <c r="W29" s="5" t="s">
         <v>181</v>
       </c>
@@ -11643,7 +11643,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="30" spans="23:94">
+    <row r="30" spans="23:94" x14ac:dyDescent="0.35">
       <c r="W30" s="5" t="s">
         <v>181</v>
       </c>
@@ -11687,7 +11687,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="31" spans="23:94">
+    <row r="31" spans="23:94" x14ac:dyDescent="0.35">
       <c r="W31" s="5" t="s">
         <v>181</v>
       </c>
@@ -11731,7 +11731,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="32" spans="23:94">
+    <row r="32" spans="23:94" x14ac:dyDescent="0.35">
       <c r="W32" s="5" t="s">
         <v>181</v>
       </c>
@@ -11775,7 +11775,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="33" spans="23:94">
+    <row r="33" spans="23:94" x14ac:dyDescent="0.35">
       <c r="W33" s="5" t="s">
         <v>181</v>
       </c>
@@ -11819,7 +11819,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="34" spans="23:94">
+    <row r="34" spans="23:94" x14ac:dyDescent="0.35">
       <c r="W34" s="5" t="s">
         <v>181</v>
       </c>
@@ -11863,7 +11863,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="35" spans="23:94">
+    <row r="35" spans="23:94" x14ac:dyDescent="0.35">
       <c r="W35" s="5" t="s">
         <v>181</v>
       </c>
@@ -12030,56 +12030,56 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" customWidth="1"/>
-    <col min="5" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" customWidth="1"/>
-    <col min="10" max="10" width="23.7109375" customWidth="1"/>
-    <col min="11" max="11" width="40.7109375" customWidth="1"/>
-    <col min="12" max="16" width="12.7109375" customWidth="1"/>
-    <col min="17" max="18" width="23.7109375" customWidth="1"/>
-    <col min="19" max="19" width="50.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" customWidth="1"/>
+    <col min="2" max="2" width="50.7265625" customWidth="1"/>
+    <col min="3" max="3" width="26.7265625" customWidth="1"/>
+    <col min="4" max="4" width="32.7265625" customWidth="1"/>
+    <col min="5" max="6" width="12.7265625" customWidth="1"/>
+    <col min="7" max="7" width="4.7265625" customWidth="1"/>
+    <col min="8" max="8" width="12.7265625" customWidth="1"/>
+    <col min="9" max="9" width="20.7265625" customWidth="1"/>
+    <col min="10" max="10" width="23.7265625" customWidth="1"/>
+    <col min="11" max="11" width="40.7265625" customWidth="1"/>
+    <col min="12" max="16" width="12.7265625" customWidth="1"/>
+    <col min="17" max="18" width="23.7265625" customWidth="1"/>
+    <col min="19" max="19" width="50.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="23.25">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:19" ht="23" x14ac:dyDescent="0.5">
+      <c r="A1" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="41"/>
+      <c r="B1" s="43"/>
       <c r="C1" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="51" t="s">
         <v>386</v>
       </c>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="49"/>
-      <c r="S1" s="49"/>
-    </row>
-    <row r="2" spans="1:19" ht="39">
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51"/>
+    </row>
+    <row r="2" spans="1:19" ht="26.5" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>120</v>
       </c>
@@ -12138,7 +12138,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="114.75">
+    <row r="3" spans="1:19" ht="112.5" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>169</v>
       </c>
@@ -12191,7 +12191,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="114.75">
+    <row r="4" spans="1:19" ht="112.5" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>169</v>
       </c>
@@ -12240,7 +12240,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="114.75">
+    <row r="5" spans="1:19" ht="112.5" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>169</v>
       </c>
@@ -12293,7 +12293,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="114.75">
+    <row r="6" spans="1:19" ht="112.5" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>169</v>
       </c>
@@ -12346,7 +12346,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="114.75">
+    <row r="7" spans="1:19" ht="112.5" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>169</v>
       </c>
@@ -12393,7 +12393,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="114.75">
+    <row r="8" spans="1:19" ht="112.5" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>169</v>
       </c>
@@ -12432,7 +12432,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="114.75">
+    <row r="9" spans="1:19" ht="112.5" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>169</v>
       </c>
@@ -12504,54 +12504,54 @@
       <selection activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="3" width="52.7109375" customWidth="1"/>
-    <col min="4" max="4" width="110.7109375" customWidth="1"/>
-    <col min="5" max="5" width="2.7109375" customWidth="1"/>
+    <col min="1" max="1" width="2.7265625" customWidth="1"/>
+    <col min="2" max="2" width="40.7265625" customWidth="1"/>
+    <col min="3" max="3" width="52.7265625" customWidth="1"/>
+    <col min="4" max="4" width="110.7265625" customWidth="1"/>
+    <col min="5" max="5" width="2.7265625" customWidth="1"/>
     <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23.25" customHeight="1">
-      <c r="B1" s="35" t="s">
+    <row r="1" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="35"/>
+      <c r="C1" s="36"/>
       <c r="D1" s="19" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="41.25" customHeight="1">
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
+    <row r="2" spans="1:5" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
       <c r="D2" s="20" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
     </row>
-    <row r="5" spans="1:5" ht="18">
-      <c r="B5" s="51" t="s">
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.4">
+      <c r="B5" s="39" t="s">
         <v>439</v>
       </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="B6" s="36" t="s">
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B6" s="37" t="s">
         <v>440</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>441</v>
       </c>
@@ -12562,7 +12562,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" s="5" t="s">
         <v>444</v>
       </c>
@@ -12573,7 +12573,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="25.5">
+    <row r="10" spans="1:5" ht="25" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
         <v>38</v>
       </c>
@@ -12584,7 +12584,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="25.5">
+    <row r="11" spans="1:5" ht="25" x14ac:dyDescent="0.35">
       <c r="B11" s="5" t="s">
         <v>449</v>
       </c>
@@ -12595,7 +12595,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B12" s="5" t="s">
         <v>452</v>
       </c>
@@ -12606,7 +12606,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B13" s="5" t="s">
         <v>455</v>
       </c>
@@ -12617,7 +12617,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B14" s="5" t="s">
         <v>457</v>
       </c>
@@ -12626,7 +12626,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B15" s="5" t="s">
         <v>459</v>
       </c>
@@ -12637,7 +12637,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="25.5">
+    <row r="16" spans="1:5" ht="25" x14ac:dyDescent="0.35">
       <c r="B16" s="5" t="s">
         <v>462</v>
       </c>
@@ -12646,7 +12646,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="5" t="s">
         <v>464</v>
       </c>
@@ -12655,7 +12655,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" s="5" t="s">
         <v>466</v>
       </c>
@@ -12666,7 +12666,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B19" s="5" t="s">
         <v>469</v>
       </c>
@@ -12677,7 +12677,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="20" spans="2:4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B20" s="5" t="s">
         <v>472</v>
       </c>
@@ -12686,7 +12686,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="21" spans="2:4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B21" s="5" t="s">
         <v>47</v>
       </c>
@@ -12695,7 +12695,7 @@
       </c>
       <c r="D21" s="5"/>
     </row>
-    <row r="22" spans="2:4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B22" s="5" t="s">
         <v>475</v>
       </c>
@@ -12706,7 +12706,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B23" s="5" t="s">
         <v>478</v>
       </c>
@@ -12717,7 +12717,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="24" spans="2:4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B24" s="5" t="s">
         <v>481</v>
       </c>
@@ -12726,7 +12726,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="25" spans="2:4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B25" s="5" t="s">
         <v>483</v>
       </c>
@@ -12735,7 +12735,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="26" spans="2:4">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B26" s="5" t="s">
         <v>485</v>
       </c>
@@ -12746,7 +12746,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="27" spans="2:4">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B27" s="5" t="s">
         <v>488</v>
       </c>
@@ -12755,7 +12755,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="28" spans="2:4" ht="25.5">
+    <row r="28" spans="2:4" ht="25" x14ac:dyDescent="0.35">
       <c r="B28" s="5" t="s">
         <v>490</v>
       </c>
@@ -12766,7 +12766,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="29" spans="2:4">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B29" s="5" t="s">
         <v>493</v>
       </c>
@@ -12775,7 +12775,7 @@
       </c>
       <c r="D29" s="5"/>
     </row>
-    <row r="30" spans="2:4">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B30" s="5" t="s">
         <v>495</v>
       </c>
@@ -12786,7 +12786,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="31" spans="2:4">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B31" s="5" t="s">
         <v>497</v>
       </c>
@@ -12795,7 +12795,7 @@
       </c>
       <c r="D31" s="5"/>
     </row>
-    <row r="32" spans="2:4">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B32" s="5" t="s">
         <v>499</v>
       </c>
@@ -12806,7 +12806,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="33" spans="2:4">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B33" s="5" t="s">
         <v>501</v>
       </c>
@@ -12815,7 +12815,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="34" spans="2:4">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B34" s="5" t="s">
         <v>503</v>
       </c>
@@ -12826,7 +12826,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="35" spans="2:4">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B35" s="5" t="s">
         <v>506</v>
       </c>
@@ -12835,7 +12835,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="36" spans="2:4">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B36" s="5" t="s">
         <v>508</v>
       </c>
@@ -12846,7 +12846,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="37" spans="2:4">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B37" s="5" t="s">
         <v>71</v>
       </c>
@@ -12855,7 +12855,7 @@
       </c>
       <c r="D37" s="5"/>
     </row>
-    <row r="38" spans="2:4">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B38" s="5" t="s">
         <v>511</v>
       </c>
@@ -12864,7 +12864,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="39" spans="2:4">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B39" s="5" t="s">
         <v>513</v>
       </c>
@@ -12873,7 +12873,7 @@
       </c>
       <c r="D39" s="5"/>
     </row>
-    <row r="40" spans="2:4" ht="25.5">
+    <row r="40" spans="2:4" ht="25" x14ac:dyDescent="0.35">
       <c r="B40" s="5" t="s">
         <v>515</v>
       </c>
@@ -12884,7 +12884,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="41" spans="2:4">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B41" s="5" t="s">
         <v>518</v>
       </c>
@@ -12895,7 +12895,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="42" spans="2:4">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B42" s="5" t="s">
         <v>521</v>
       </c>
@@ -12904,7 +12904,7 @@
       </c>
       <c r="D42" s="5"/>
     </row>
-    <row r="43" spans="2:4">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B43" s="5" t="s">
         <v>523</v>
       </c>
@@ -12913,7 +12913,7 @@
       </c>
       <c r="D43" s="5"/>
     </row>
-    <row r="44" spans="2:4">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B44" s="5" t="s">
         <v>525</v>
       </c>
@@ -12924,7 +12924,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="45" spans="2:4">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B45" s="5" t="s">
         <v>528</v>
       </c>
@@ -12933,7 +12933,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="46" spans="2:4">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B46" s="5" t="s">
         <v>530</v>
       </c>
@@ -12942,7 +12942,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="47" spans="2:4">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B47" s="5" t="s">
         <v>532</v>
       </c>
@@ -12951,7 +12951,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="48" spans="2:4">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B48" s="5" t="s">
         <v>534</v>
       </c>
@@ -12960,7 +12960,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="49" spans="2:4">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B49" s="5" t="s">
         <v>536</v>
       </c>
@@ -12971,7 +12971,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="50" spans="2:4">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B50" s="5" t="s">
         <v>539</v>
       </c>
@@ -12980,7 +12980,7 @@
       </c>
       <c r="D50" s="5"/>
     </row>
-    <row r="51" spans="2:4">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B51" s="5" t="s">
         <v>541</v>
       </c>
@@ -12989,7 +12989,7 @@
       </c>
       <c r="D51" s="5"/>
     </row>
-    <row r="52" spans="2:4">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B52" s="5" t="s">
         <v>543</v>
       </c>
@@ -12998,7 +12998,7 @@
       </c>
       <c r="D52" s="5"/>
     </row>
-    <row r="53" spans="2:4">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B53" s="5" t="s">
         <v>545</v>
       </c>
@@ -13007,7 +13007,7 @@
       </c>
       <c r="D53" s="5"/>
     </row>
-    <row r="54" spans="2:4">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B54" s="5" t="s">
         <v>547</v>
       </c>
@@ -13016,7 +13016,7 @@
       </c>
       <c r="D54" s="5"/>
     </row>
-    <row r="55" spans="2:4">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B55" s="5" t="s">
         <v>549</v>
       </c>
@@ -13025,7 +13025,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="56" spans="2:4">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B56" s="5" t="s">
         <v>551</v>
       </c>
@@ -13036,7 +13036,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="57" spans="2:4">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B57" s="5" t="s">
         <v>554</v>
       </c>
@@ -13045,7 +13045,7 @@
       </c>
       <c r="D57" s="5"/>
     </row>
-    <row r="58" spans="2:4">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B58" s="5" t="s">
         <v>136</v>
       </c>
@@ -13054,7 +13054,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="59" spans="2:4">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B59" s="5" t="s">
         <v>557</v>
       </c>
@@ -13063,7 +13063,7 @@
       </c>
       <c r="D59" s="5"/>
     </row>
-    <row r="60" spans="2:4">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B60" s="5" t="s">
         <v>559</v>
       </c>
@@ -13074,7 +13074,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="61" spans="2:4">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B61" s="5" t="s">
         <v>561</v>
       </c>
@@ -13085,7 +13085,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="62" spans="2:4" ht="25.5">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B62" s="5" t="s">
         <v>564</v>
       </c>
@@ -13096,7 +13096,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="63" spans="2:4" ht="25.5">
+    <row r="63" spans="2:4" ht="25" x14ac:dyDescent="0.35">
       <c r="B63" s="5" t="s">
         <v>567</v>
       </c>
@@ -13107,7 +13107,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="64" spans="2:4" ht="25.5">
+    <row r="64" spans="2:4" ht="25" x14ac:dyDescent="0.35">
       <c r="B64" s="5" t="s">
         <v>570</v>
       </c>
@@ -13118,7 +13118,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="65" spans="2:4" ht="25.5">
+    <row r="65" spans="2:4" ht="25" x14ac:dyDescent="0.35">
       <c r="B65" s="5" t="s">
         <v>573</v>
       </c>
@@ -13129,7 +13129,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="66" spans="2:4">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B66" s="5" t="s">
         <v>576</v>
       </c>
@@ -13138,7 +13138,7 @@
       </c>
       <c r="D66" s="5"/>
     </row>
-    <row r="67" spans="2:4" ht="25.5">
+    <row r="67" spans="2:4" ht="25" x14ac:dyDescent="0.35">
       <c r="B67" s="5" t="s">
         <v>578</v>
       </c>
@@ -13149,7 +13149,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="68" spans="2:4">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B68" s="5" t="s">
         <v>581</v>
       </c>
@@ -13158,7 +13158,7 @@
       </c>
       <c r="D68" s="5"/>
     </row>
-    <row r="69" spans="2:4">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B69" s="5" t="s">
         <v>583</v>
       </c>
@@ -13169,7 +13169,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="70" spans="2:4">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B70" s="5" t="s">
         <v>586</v>
       </c>
@@ -13180,7 +13180,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="71" spans="2:4">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B71" s="5" t="s">
         <v>589</v>
       </c>
@@ -13191,7 +13191,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="72" spans="2:4">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B72" s="5" t="s">
         <v>591</v>
       </c>
@@ -13200,7 +13200,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="73" spans="2:4">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B73" s="5" t="s">
         <v>593</v>
       </c>
@@ -13209,7 +13209,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="74" spans="2:4">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B74" s="5" t="s">
         <v>595</v>
       </c>
@@ -13220,7 +13220,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="75" spans="2:4" ht="38.25">
+    <row r="75" spans="2:4" ht="37.5" x14ac:dyDescent="0.35">
       <c r="B75" s="5" t="s">
         <v>597</v>
       </c>
@@ -13229,7 +13229,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="76" spans="2:4">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B76" s="5" t="s">
         <v>599</v>
       </c>
@@ -13240,7 +13240,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="77" spans="2:4">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B77" s="5" t="s">
         <v>602</v>
       </c>
@@ -13251,7 +13251,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="78" spans="2:4" ht="25.5">
+    <row r="78" spans="2:4" ht="25" x14ac:dyDescent="0.35">
       <c r="B78" s="5" t="s">
         <v>605</v>
       </c>
@@ -13260,7 +13260,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="79" spans="2:4" ht="25.5">
+    <row r="79" spans="2:4" ht="25" x14ac:dyDescent="0.35">
       <c r="B79" s="5" t="s">
         <v>607</v>
       </c>
@@ -13269,7 +13269,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="80" spans="2:4">
+    <row r="80" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B80" s="5" t="s">
         <v>609</v>
       </c>
@@ -13278,7 +13278,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="81" spans="2:4">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B81" s="5" t="s">
         <v>611</v>
       </c>
@@ -13287,7 +13287,7 @@
       </c>
       <c r="D81" s="5"/>
     </row>
-    <row r="82" spans="2:4">
+    <row r="82" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B82" s="5" t="s">
         <v>613</v>
       </c>
@@ -13298,7 +13298,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="83" spans="2:4">
+    <row r="83" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B83" s="5" t="s">
         <v>616</v>
       </c>
@@ -13307,7 +13307,7 @@
       </c>
       <c r="D83" s="5"/>
     </row>
-    <row r="84" spans="2:4">
+    <row r="84" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B84" s="5" t="s">
         <v>618</v>
       </c>
@@ -13316,7 +13316,7 @@
       </c>
       <c r="D84" s="5"/>
     </row>
-    <row r="85" spans="2:4">
+    <row r="85" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B85" s="5" t="s">
         <v>620</v>
       </c>
@@ -13347,54 +13347,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <i8d248d2f27048728597da4d9cc9bde9 xmlns="60b4899e-55b4-4231-8241-12d69350e134" xsi:nil="true"/>
-    <TaxCatchAll xmlns="d65852a7-7f3c-4f0b-a9f7-42acedd46965">
-      <Value>3</Value>
-      <Value>2</Value>
-      <Value>1</Value>
-    </TaxCatchAll>
-    <ie640504e2964b25856743efbfa846d6 xmlns="60b4899e-55b4-4231-8241-12d69350e134">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Crown</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">69589897-2828-4761-976e-717fd8e631c9</TermId>
-        </TermInfo>
-      </Terms>
-    </ie640504e2964b25856743efbfa846d6>
-    <id2a76e1917c4be6961e12b425f79256 xmlns="60b4899e-55b4-4231-8241-12d69350e134">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">DDaT Data Services and Analytics (DSA)</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">f0cba11e-b0b0-428b-840c-a0397e397bd6</TermId>
-        </TermInfo>
-      </Terms>
-    </id2a76e1917c4be6961e12b425f79256>
-    <HOMigrated xmlns="60b4899e-55b4-4231-8241-12d69350e134">false</HOMigrated>
-    <lae2bfa7b6474897ab4a53f76ea236c7 xmlns="d65852a7-7f3c-4f0b-a9f7-42acedd46965">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Official</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">14c80daa-741b-422c-9722-f71693c9ede4</TermId>
-        </TermInfo>
-      </Terms>
-    </lae2bfa7b6474897ab4a53f76ea236c7>
-    <HOworkspaceType xmlns="60b4899e-55b4-4231-8241-12d69350e134">Continuous Teamwork</HOworkspaceType>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="HO document" ma:contentTypeID="0x010100A5BF1C78D9F64B679A5EBDE1C6598EBC0100C97B8F48964F80438FF61D0E8AF9793B" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="03b4dd9600bc57512658a5f1042ed315">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="60b4899e-55b4-4231-8241-12d69350e134" xmlns:ns3="d65852a7-7f3c-4f0b-a9f7-42acedd46965" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e02dc6de035cee5c7075b2538af8c9bd" ns2:_="" ns3:_="">
     <xsd:import namespace="60b4899e-55b4-4231-8241-12d69350e134"/>
@@ -13585,14 +13537,88 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <i8d248d2f27048728597da4d9cc9bde9 xmlns="60b4899e-55b4-4231-8241-12d69350e134" xsi:nil="true"/>
+    <TaxCatchAll xmlns="d65852a7-7f3c-4f0b-a9f7-42acedd46965">
+      <Value>3</Value>
+      <Value>2</Value>
+      <Value>1</Value>
+    </TaxCatchAll>
+    <ie640504e2964b25856743efbfa846d6 xmlns="60b4899e-55b4-4231-8241-12d69350e134">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Crown</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">69589897-2828-4761-976e-717fd8e631c9</TermId>
+        </TermInfo>
+      </Terms>
+    </ie640504e2964b25856743efbfa846d6>
+    <id2a76e1917c4be6961e12b425f79256 xmlns="60b4899e-55b4-4231-8241-12d69350e134">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">DDaT Data Services and Analytics (DSA)</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">f0cba11e-b0b0-428b-840c-a0397e397bd6</TermId>
+        </TermInfo>
+      </Terms>
+    </id2a76e1917c4be6961e12b425f79256>
+    <HOMigrated xmlns="60b4899e-55b4-4231-8241-12d69350e134">false</HOMigrated>
+    <lae2bfa7b6474897ab4a53f76ea236c7 xmlns="d65852a7-7f3c-4f0b-a9f7-42acedd46965">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Official</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">14c80daa-741b-422c-9722-f71693c9ede4</TermId>
+        </TermInfo>
+      </Terms>
+    </lae2bfa7b6474897ab4a53f76ea236c7>
+    <HOworkspaceType xmlns="60b4899e-55b4-4231-8241-12d69350e134">Continuous Teamwork</HOworkspaceType>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49A847CD-6E28-4010-AF49-D113EAC15B79}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E9B24F-C72B-4407-A876-BF563AB59E45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="60b4899e-55b4-4231-8241-12d69350e134"/>
+    <ds:schemaRef ds:uri="d65852a7-7f3c-4f0b-a9f7-42acedd46965"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03DAF9A5-54FD-43EE-8958-89E80EA4552E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49A847CD-6E28-4010-AF49-D113EAC15B79}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E9B24F-C72B-4407-A876-BF563AB59E45}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03DAF9A5-54FD-43EE-8958-89E80EA4552E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="60b4899e-55b4-4231-8241-12d69350e134"/>
+    <ds:schemaRef ds:uri="d65852a7-7f3c-4f0b-a9f7-42acedd46965"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>